<commit_message>
Atualização automática de TRES_DE_MAIO.xlsx
</commit_message>
<xml_diff>
--- a/TRES_DE_MAIO.xlsx
+++ b/TRES_DE_MAIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71C226A2-0B17-439F-B02A-2A4BF4243849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8292E9D-9BD7-4A68-842E-D30FEBF1E6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1276,7 +1276,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{5B569410-EEF4-4DFB-834E-F5C36D215B61}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{8E999321-A5E3-4DB6-98CE-55E7C80E4217}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1306,10 +1306,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27ABC031-E075-4949-A2F1-0CA12CFFD719}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3763C12D-6712-4A1B-9D85-B96299F97D65}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1347,7 +1347,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F853912C-AF74-44C7-9CCA-6AF8CD3F680B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E03EDD-F322-4C3D-8346-1D7167B8EB02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1410,7 +1410,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAB40460-77CB-4156-BC41-BDC1ED7698BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E3AA3F6-84E0-46C1-8010-738D0DACA030}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1429,7 +1429,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2123BC79-F9ED-A448-48E9-22814A22C1C0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87AC4FA4-B0EF-9196-F70A-43773674C8A8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1478,7 +1478,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91D7315B-CF9A-8BE7-613A-7375C9B9D678}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D257C12-FB32-22BA-14C0-E67B28C9999B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1497,7 +1497,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E4B98C-9B12-973C-41B9-59F4038866B8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4494F10B-B65C-8422-A734-194ABC0A102D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1528,7 +1528,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2DB07F9-AA94-ACDF-333A-2551531C8C88}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2112EF6C-3BA1-31C1-8E98-E9F819303DBF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1559,7 +1559,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5657EDC-FEEB-E4AA-F7CB-035C53AE0D05}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B92FB7-44D0-8379-6968-9810FA3E2141}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1602,7 +1602,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BFCB4A3-5F3A-4168-8A26-AD45B1B26D30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98F5614B-EFB4-4362-B83D-FD78A001A65F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1640,7 +1640,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{060046D3-6386-49C7-B725-AAD38FF76665}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D12B40A-ABE6-40CC-B681-B542EC269305}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1683,7 +1683,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F349F96-D90E-49DF-B92F-9643D26D7342}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{265F531A-AFAD-4E08-8CAB-DF242ADA793C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1996,7 +1996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F00AE8D-94D8-4CDC-9C43-D8DFF48B861F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2658C0EE-4F3E-4BD2-9557-CAC531B2FB3C}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>